<commit_message>
[ELAB-400] updated current findings about Splunk
</commit_message>
<xml_diff>
--- a/data/Tools-und-Werkzeuge.xlsx
+++ b/data/Tools-und-Werkzeuge.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\bachelorarbeit\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A6D2461-C9B7-4FDB-A26F-95FA14A43C27}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{861D9DE3-493B-4FD6-A80A-F507AE24BEFC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1020" windowWidth="28770" windowHeight="13080" xr2:uid="{97483665-8731-4B46-80DA-A5AC37BBF732}"/>
+    <workbookView xWindow="6" yWindow="6" windowWidth="23028" windowHeight="12948" xr2:uid="{97483665-8731-4B46-80DA-A5AC37BBF732}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -211,7 +211,55 @@
         </r>
       </text>
     </comment>
-    <comment ref="G11" authorId="0" shapeId="0" xr:uid="{C363115E-6B1F-4C7C-8853-F7948B710482}">
+    <comment ref="C7" authorId="0" shapeId="0" xr:uid="{CEAC94EF-C443-4D7C-A9F4-4D5B3F62F554}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t>Marvin Kienitz:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Das APM ist nicht so detailreich wie bei "richtigen" APMs und richtet sich mehr auf System/Infrastruktur Monitoring</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F7" authorId="0" shapeId="0" xr:uid="{F980FF3B-428D-4F24-A6FC-0DCA8387BA9F}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t>Marvin Kienitz:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Ein Error Monitoring ist vorhanden, aber es gibt keine direkte Einsicht in die eigentlichen Fehler, sondern eher in den Zusammenhang mit der Infrastruktur. Dies lässt die nachfolgende Suche zur Fehlerursache besser einschränken, aber ersetzt diese Suche nicht.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G12" authorId="0" shapeId="0" xr:uid="{C363115E-6B1F-4C7C-8853-F7948B710482}">
       <text>
         <r>
           <rPr>
@@ -235,7 +283,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I11" authorId="0" shapeId="0" xr:uid="{7F0EB4C8-729B-47F8-9E69-5B0E61196DD3}">
+    <comment ref="I12" authorId="0" shapeId="0" xr:uid="{7F0EB4C8-729B-47F8-9E69-5B0E61196DD3}">
       <text>
         <r>
           <rPr>
@@ -264,7 +312,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="57">
   <si>
     <t>Sentry</t>
   </si>
@@ -433,6 +481,17 @@
   <si>
     <t xml:space="preserve"> - erlaubt kein direktes Senden von Logs vom Browser aus
  - verfügbar als On-Premise</t>
+  </si>
+  <si>
+    <t>Splunk APM
+ (SignalFX)</t>
+  </si>
+  <si>
+    <t>https://www.splunk.com/en_us/software/splunk-apm.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - erlaubt kein direktes Senden von Logs vom Browser aus
+ - optimiert für Cloud-Anwendungen (aber auch OnPremise und hybride)</t>
   </si>
 </sst>
 </file>
@@ -690,7 +749,7 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
@@ -725,6 +784,12 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="6" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="6" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
@@ -1046,10 +1111,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B100F075-474E-4DC4-B7D3-5AD823E768A3}">
-  <dimension ref="A1:K19"/>
+  <dimension ref="A1:K20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I9:I10"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1209,104 +1274,102 @@
         <v>43</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" ht="32.25" x14ac:dyDescent="0.3">
       <c r="A7" s="4"/>
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="G7" s="16"/>
+      <c r="H7" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="I7" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="K7" s="28" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A8" s="4"/>
+      <c r="B8" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="14" t="s">
+      <c r="C8" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="14" t="s">
+      <c r="D8" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="E7" s="9"/>
-      <c r="F7" s="14" t="s">
+      <c r="E8" s="9"/>
+      <c r="F8" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="G7" s="14" t="s">
+      <c r="G8" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="H7" s="17"/>
-      <c r="I7" s="14" t="s">
+      <c r="H8" s="17"/>
+      <c r="I8" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="J7" s="2" t="s">
+      <c r="J8" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="K7" s="25" t="s">
+      <c r="K8" s="25" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A8" s="5"/>
-      <c r="B8" s="13" t="s">
+    <row r="9" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A9" s="5"/>
+      <c r="B9" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="C8" s="26" t="s">
+      <c r="C9" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="26"/>
-      <c r="E8" s="26"/>
-      <c r="F8" s="26"/>
-      <c r="G8" s="26"/>
-      <c r="H8" s="26"/>
-      <c r="I8" s="26"/>
-      <c r="J8" s="3" t="s">
+      <c r="D9" s="26"/>
+      <c r="E9" s="26"/>
+      <c r="F9" s="26"/>
+      <c r="G9" s="26"/>
+      <c r="H9" s="26"/>
+      <c r="I9" s="26"/>
+      <c r="J9" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="K8" s="25" t="s">
+      <c r="K9" s="25" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A9" s="22" t="s">
+    <row r="10" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A10" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="19"/>
-      <c r="C9" s="20"/>
-      <c r="D9" s="20"/>
-      <c r="E9" s="20"/>
-      <c r="F9" s="20"/>
-      <c r="G9" s="20"/>
-      <c r="H9" s="20"/>
-      <c r="I9" s="20"/>
-      <c r="J9" s="20"/>
-      <c r="K9" s="20"/>
-    </row>
-    <row r="10" spans="1:11" ht="45.75" x14ac:dyDescent="0.3">
-      <c r="A10" s="4"/>
-      <c r="B10" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="C10" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="D10" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="E10" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="F10" s="9"/>
-      <c r="G10" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="H10" s="16"/>
-      <c r="I10" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="J10" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="K10" s="25" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" ht="30.75" x14ac:dyDescent="0.3">
+      <c r="B10" s="19"/>
+      <c r="C10" s="20"/>
+      <c r="D10" s="20"/>
+      <c r="E10" s="20"/>
+      <c r="F10" s="20"/>
+      <c r="G10" s="20"/>
+      <c r="H10" s="20"/>
+      <c r="I10" s="20"/>
+      <c r="J10" s="20"/>
+      <c r="K10" s="20"/>
+    </row>
+    <row r="11" spans="1:11" ht="45.75" x14ac:dyDescent="0.3">
       <c r="A11" s="4"/>
       <c r="B11" s="10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C11" s="12" t="s">
         <v>9</v>
@@ -1326,37 +1389,45 @@
         <v>9</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="K11" s="25" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="30.75" x14ac:dyDescent="0.3">
       <c r="A12" s="4"/>
       <c r="B12" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="D12" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E12" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="F12" s="9"/>
+      <c r="G12" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="H12" s="16"/>
+      <c r="I12" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="J12" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="K12" s="25" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A13" s="4"/>
+      <c r="B13" s="10" t="s">
         <v>13</v>
-      </c>
-      <c r="C12" s="26" t="s">
-        <v>15</v>
-      </c>
-      <c r="D12" s="26"/>
-      <c r="E12" s="26"/>
-      <c r="F12" s="26"/>
-      <c r="G12" s="26"/>
-      <c r="H12" s="26"/>
-      <c r="I12" s="26"/>
-      <c r="J12" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="K12" s="25" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A13" s="5"/>
-      <c r="B13" s="13" t="s">
-        <v>14</v>
       </c>
       <c r="C13" s="26" t="s">
         <v>15</v>
@@ -1371,81 +1442,81 @@
         <v>19</v>
       </c>
       <c r="K13" s="25" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A14" s="5"/>
+      <c r="B14" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="D14" s="26"/>
+      <c r="E14" s="26"/>
+      <c r="F14" s="26"/>
+      <c r="G14" s="26"/>
+      <c r="H14" s="26"/>
+      <c r="I14" s="26"/>
+      <c r="J14" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K14" s="25" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A14" s="22" t="s">
+    <row r="15" spans="1:11" ht="46.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="B14" s="19"/>
-      <c r="C14" s="20"/>
-      <c r="D14" s="20"/>
-      <c r="E14" s="20"/>
-      <c r="F14" s="20"/>
-      <c r="G14" s="20"/>
-      <c r="H14" s="20"/>
-      <c r="I14" s="20"/>
-      <c r="J14" s="20"/>
-      <c r="K14" s="21"/>
-    </row>
-    <row r="15" spans="1:11" ht="46.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="4"/>
-      <c r="B15" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="C15" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="D15" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="E15" s="9"/>
-      <c r="F15" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="G15" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="H15" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="I15" s="9"/>
-      <c r="J15" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="K15" s="25" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B15" s="19"/>
+      <c r="C15" s="20"/>
+      <c r="D15" s="20"/>
+      <c r="E15" s="20"/>
+      <c r="F15" s="20"/>
+      <c r="G15" s="20"/>
+      <c r="H15" s="20"/>
+      <c r="I15" s="20"/>
+      <c r="J15" s="20"/>
+      <c r="K15" s="21"/>
+    </row>
+    <row r="16" spans="1:11" ht="60.75" x14ac:dyDescent="0.3">
       <c r="A16" s="4"/>
       <c r="B16" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="C16" s="26" t="s">
-        <v>26</v>
-      </c>
-      <c r="D16" s="26"/>
-      <c r="E16" s="26"/>
-      <c r="F16" s="26"/>
-      <c r="G16" s="26"/>
-      <c r="H16" s="26"/>
-      <c r="I16" s="26"/>
-      <c r="J16" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="K16" s="24" t="s">
-        <v>52</v>
+        <v>18</v>
+      </c>
+      <c r="C16" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="D16" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="E16" s="9"/>
+      <c r="F16" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="G16" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="H16" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="I16" s="9"/>
+      <c r="J16" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="K16" s="25" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A17" s="4"/>
       <c r="B17" s="10" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C17" s="26" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D17" s="26"/>
       <c r="E17" s="26"/>
@@ -1463,28 +1534,28 @@
     <row r="18" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A18" s="4"/>
       <c r="B18" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C18" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="D18" s="26"/>
+      <c r="E18" s="26"/>
+      <c r="F18" s="26"/>
+      <c r="G18" s="26"/>
+      <c r="H18" s="26"/>
+      <c r="I18" s="26"/>
+      <c r="J18" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K18" s="24" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A19" s="4"/>
+      <c r="B19" s="10" t="s">
         <v>32</v>
-      </c>
-      <c r="C18" s="15"/>
-      <c r="D18" s="15"/>
-      <c r="E18" s="15"/>
-      <c r="F18" s="15"/>
-      <c r="G18" s="15"/>
-      <c r="H18" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="I18" s="15"/>
-      <c r="J18" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="K18" s="25" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A19" s="5"/>
-      <c r="B19" s="13" t="s">
-        <v>33</v>
       </c>
       <c r="C19" s="15"/>
       <c r="D19" s="15"/>
@@ -1499,33 +1570,55 @@
         <v>35</v>
       </c>
       <c r="K19" s="25" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A20" s="5"/>
+      <c r="B20" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="C20" s="15"/>
+      <c r="D20" s="15"/>
+      <c r="E20" s="15"/>
+      <c r="F20" s="15"/>
+      <c r="G20" s="15"/>
+      <c r="H20" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="I20" s="15"/>
+      <c r="J20" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="K20" s="25" t="s">
         <v>51</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="C8:I8"/>
+    <mergeCell ref="C9:I9"/>
+    <mergeCell ref="C14:I14"/>
     <mergeCell ref="C13:I13"/>
-    <mergeCell ref="C12:I12"/>
-    <mergeCell ref="C16:I16"/>
     <mergeCell ref="C17:I17"/>
+    <mergeCell ref="C18:I18"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="K3" r:id="rId1" xr:uid="{C3305201-657E-477C-ACEE-77E4CC876A74}"/>
     <hyperlink ref="K4" r:id="rId2" xr:uid="{26436B73-C6BA-4412-A904-EBFFAF46428B}"/>
-    <hyperlink ref="K6" r:id="rId3" xr:uid="{A9AA41D7-8125-4A0E-8786-EA05A4FA0CB1}"/>
-    <hyperlink ref="K7" r:id="rId4" xr:uid="{30B94C73-A6A0-47CC-8FE9-EF51F2E473CF}"/>
-    <hyperlink ref="K8" r:id="rId5" xr:uid="{DE7EB6C8-626F-4D42-81D3-F4A2F7A09886}"/>
-    <hyperlink ref="K10" r:id="rId6" xr:uid="{A5023D41-05E6-4977-BE28-0106456D6CA3}"/>
-    <hyperlink ref="K11" r:id="rId7" xr:uid="{9A3BD5FA-F460-4DE8-8775-3D31A94BEA8C}"/>
-    <hyperlink ref="K12" r:id="rId8" xr:uid="{8ABF9867-7EA7-468B-8B94-596EC770FB75}"/>
-    <hyperlink ref="K13" r:id="rId9" xr:uid="{025F4242-BE8B-4382-87E7-0302D8A50D1E}"/>
-    <hyperlink ref="K15" r:id="rId10" xr:uid="{5F33EF71-DBDE-42C6-ABAD-0DCA4479747B}"/>
-    <hyperlink ref="K18" r:id="rId11" xr:uid="{5528CEDB-B63D-4B8B-BFF0-94D7F517006D}"/>
-    <hyperlink ref="K19" r:id="rId12" xr:uid="{EE879F8C-5A60-4315-BEA9-83F4CC3E7EB5}"/>
+    <hyperlink ref="K7" r:id="rId3" xr:uid="{A9AA41D7-8125-4A0E-8786-EA05A4FA0CB1}"/>
+    <hyperlink ref="K8" r:id="rId4" xr:uid="{30B94C73-A6A0-47CC-8FE9-EF51F2E473CF}"/>
+    <hyperlink ref="K9" r:id="rId5" xr:uid="{DE7EB6C8-626F-4D42-81D3-F4A2F7A09886}"/>
+    <hyperlink ref="K11" r:id="rId6" xr:uid="{A5023D41-05E6-4977-BE28-0106456D6CA3}"/>
+    <hyperlink ref="K12" r:id="rId7" xr:uid="{9A3BD5FA-F460-4DE8-8775-3D31A94BEA8C}"/>
+    <hyperlink ref="K13" r:id="rId8" xr:uid="{8ABF9867-7EA7-468B-8B94-596EC770FB75}"/>
+    <hyperlink ref="K14" r:id="rId9" xr:uid="{025F4242-BE8B-4382-87E7-0302D8A50D1E}"/>
+    <hyperlink ref="K16" r:id="rId10" xr:uid="{5F33EF71-DBDE-42C6-ABAD-0DCA4479747B}"/>
+    <hyperlink ref="K19" r:id="rId11" xr:uid="{5528CEDB-B63D-4B8B-BFF0-94D7F517006D}"/>
+    <hyperlink ref="K20" r:id="rId12" xr:uid="{EE879F8C-5A60-4315-BEA9-83F4CC3E7EB5}"/>
+    <hyperlink ref="K6" r:id="rId13" xr:uid="{0DC2F1AD-4FE6-4B1B-B3F3-A44205805CC5}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId13"/>
-  <legacyDrawing r:id="rId14"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId14"/>
+  <legacyDrawing r:id="rId15"/>
 </worksheet>
 </file>
</xml_diff>